<commit_message>
wk 2 formatting data exercise
Added metadata to cleaned data set after talking about what it is with Shawn. Notes on column type and specific data entries added to a second tab/spreadsheet explaining the cleaned data.
</commit_message>
<xml_diff>
--- a/wk 2 formatting data exercise.xlsx
+++ b/wk 2 formatting data exercise.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="cleaned data" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="65">
   <si>
     <t>Dwelling</t>
   </si>
@@ -109,13 +109,115 @@
   </si>
   <si>
     <t>sunbricks</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Study looking at dwellings, plots, livestocks and water use for farms in Mozambique and Tanzania.</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Key ID</t>
+  </si>
+  <si>
+    <t>ID attached to each farm surveyed. 1-20 for Mozambique and Tanzania.</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Country in which farm is</t>
+  </si>
+  <si>
+    <t>What the roof is made from</t>
+  </si>
+  <si>
+    <t>What materials the floor is made from</t>
+  </si>
+  <si>
+    <t>What materials the walls are made from</t>
+  </si>
+  <si>
+    <t>The number of rooms in each dwelling</t>
+  </si>
+  <si>
+    <t>Includes cowshed on farm (yes/no)</t>
+  </si>
+  <si>
+    <t>Includes barn on farm (yes/no)</t>
+  </si>
+  <si>
+    <t>Data shows there is livestock but it is not specified or ther are disrepancies in data (ie. number implied but not listed as a specific listed animal)</t>
+  </si>
+  <si>
+    <t>Number of oxen</t>
+  </si>
+  <si>
+    <t>Number of poultry</t>
+  </si>
+  <si>
+    <t>Number of goats</t>
+  </si>
+  <si>
+    <t>Number of cows</t>
+  </si>
+  <si>
+    <t>Number of plots on farm</t>
+  </si>
+  <si>
+    <t>Data for water use but does not specify if there is a specific time of year, maybe suggests it is all year.</t>
+  </si>
+  <si>
+    <t>Water use only in summer</t>
+  </si>
+  <si>
+    <t>Data Entries</t>
+  </si>
+  <si>
+    <t>Blank cells</t>
+  </si>
+  <si>
+    <t>Row 12, columns I-M</t>
+  </si>
+  <si>
+    <t>Row 11, column N</t>
+  </si>
+  <si>
+    <t>Row 22</t>
+  </si>
+  <si>
+    <t>Key ID's 11-20</t>
+  </si>
+  <si>
+    <t>No data provided on plots. Left blank for missing data.</t>
+  </si>
+  <si>
+    <t>Data for key ID 20 only collected on dwelling. Livestock and plots and water use not included. Left blank for missing data.</t>
+  </si>
+  <si>
+    <t>No data provided. Left blank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blank data for key ID 10. No data on livestock provided. Left blank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data was missing. Left blank. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +228,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -167,14 +278,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,29 +618,29 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -579,16 +699,16 @@
       <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -629,16 +749,16 @@
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -679,16 +799,16 @@
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
@@ -727,16 +847,16 @@
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -777,16 +897,16 @@
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -827,16 +947,16 @@
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -877,16 +997,16 @@
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -927,16 +1047,16 @@
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -977,16 +1097,16 @@
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1025,16 +1145,16 @@
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>5</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1061,16 +1181,16 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>2</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1105,16 +1225,16 @@
       <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1149,16 +1269,16 @@
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1193,16 +1313,16 @@
       <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1237,16 +1357,16 @@
       <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>2</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1281,16 +1401,16 @@
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1325,16 +1445,16 @@
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1369,16 +1489,16 @@
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1413,16 +1533,16 @@
       <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1457,16 +1577,16 @@
       <c r="B22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1496,13 +1616,217 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="49" style="5" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>